<commit_message>
re framework 기초_수정중 0401
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ICT CoC\Documents\UiPath\001_ACME\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2806B5A4-2391-4127-AE70-D1750CB378B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4498A7DB-225A-4721-BE2E-5D2C0EBD788D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -192,6 +192,22 @@
   </si>
   <si>
     <t>WorkItemsUpDate_Url</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>AllKill대상</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t xml:space="preserve">구분자| </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>excel|iexplore|chrome|msedge</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>시스템에러 몇번일때 다시 처음부터 시작할 것인지?</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -199,7 +215,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -222,6 +238,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -250,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -262,6 +285,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -579,7 +603,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -690,7 +714,17 @@
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1685,7 +1719,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1741,7 +1775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="45.75">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1750,6 +1784,9 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>34</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>